<commit_message>
Final production ready code (dummy data)
</commit_message>
<xml_diff>
--- a/backend/data/stocks.xlsx
+++ b/backend/data/stocks.xlsx
@@ -6,6 +6,7 @@
     <sheet name="doors" sheetId="1" r:id="rId1"/>
     <sheet name="sunmica" sheetId="2" r:id="rId2"/>
     <sheet name="plywood" sheetId="3" r:id="rId3"/>
+    <sheet name="hardware" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -428,9 +429,17 @@
         <v>40</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>d003</v>
+      </c>
+      <c r="B4">
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -501,7 +510,7 @@
         <v>p002</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>-10</v>
       </c>
     </row>
   </sheetData>
@@ -509,4 +518,34 @@
     <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>stock</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Hardware 1mm</v>
+      </c>
+      <c r="B2">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>